<commit_message>
att banco de dados e site
</commit_message>
<xml_diff>
--- a/Backlog_projeto_individual.xlsx
+++ b/Backlog_projeto_individual.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15a7ca5f30cd3020/Desktop/Github-Projetos/Andrei/Projeto_Individual/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive\Desktop\Github-Projetos\Andrei\Projeto_Individual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="514" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DC025F8-C502-403A-95EE-011328F1A88F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FEAC60-A7DE-4F2C-869B-BD342CF57A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="67">
   <si>
     <t>Requisito</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Documentação do projeto</t>
+  </si>
+  <si>
+    <t>Linkar o tema do projeto com algum objetivo de desenvolvimento sustentável( ODS) da ONU</t>
   </si>
 </sst>
 </file>
@@ -244,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-416]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +257,14 @@
     </font>
     <font>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -280,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -317,6 +328,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,7 +596,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>419</c:v>
+                  <c:v>424</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>79</c:v>
@@ -593,7 +608,7 @@
                   <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>89</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -661,13 +676,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>87</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1797,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1884,11 +1899,11 @@
       </c>
       <c r="N2">
         <f>SUM(N3:N6)</f>
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="O2">
         <f>SUM(O3:O6)</f>
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1960,7 +1975,7 @@
       </c>
       <c r="O4">
         <f>SUMPRODUCT(SUMIFS($F$2:$F$36,$H$2:$H$36,M4,$I$2:$I$36,TRUE))</f>
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2025,15 +2040,16 @@
       <c r="I6" s="6" t="b">
         <v>1</v>
       </c>
+      <c r="K6" s="12"/>
       <c r="M6" s="7">
         <v>45985</v>
       </c>
       <c r="N6">
-        <f>SUMPRODUCT(SUMIFS($F$2:$F$36,$H$2:$H$36,M6))</f>
-        <v>89</v>
+        <f>SUMPRODUCT(SUMIFS($F$2:$F$37,$H$2:$H$37,M6))</f>
+        <v>94</v>
       </c>
       <c r="O6">
-        <f>SUMPRODUCT(SUMIFS($F$2:$F$36,$H$2:$H$36,M6,$I$2:$I$36,TRUE))</f>
+        <f>SUMPRODUCT(SUMIFS($F$2:$F$37,$H$2:$H$37,M6,$I$2:$I$37,TRUE))</f>
         <v>0</v>
       </c>
     </row>
@@ -2068,11 +2084,11 @@
       </c>
       <c r="N7">
         <f>AVERAGE(N3:N6)</f>
-        <v>104.75</v>
+        <v>106</v>
       </c>
       <c r="O7">
         <f>AVERAGE(O3:O6)</f>
-        <v>21.75</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2128,7 +2144,7 @@
         <v>45971</v>
       </c>
       <c r="I9" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -2761,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
       <c r="B34" s="8"/>
       <c r="C34" s="4" t="s">
@@ -2836,19 +2852,44 @@
         <v>0</v>
       </c>
     </row>
+    <row r="37" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="9"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="4">
+        <v>5</v>
+      </c>
+      <c r="G37" s="4">
+        <v>1</v>
+      </c>
+      <c r="H37" s="11">
+        <v>45985</v>
+      </c>
+      <c r="I37" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="B28:B31"/>
-    <mergeCell ref="B32:B36"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A24"/>
     <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A32:A36"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B12:B18"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="A32:A37"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="containsText" dxfId="10" priority="21" operator="containsText" text="Desejável">

</xml_diff>

<commit_message>
Commit com compressão de video
</commit_message>
<xml_diff>
--- a/Backlog_projeto_individual.xlsx
+++ b/Backlog_projeto_individual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15a7ca5f30cd3020/Desktop/Github-Projetos/Andrei/Projeto_Individual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{44FEAC60-A7DE-4F2C-869B-BD342CF57A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{650058F3-CD69-408F-92A2-FE8E891ABCC3}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{44FEAC60-A7DE-4F2C-869B-BD342CF57A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5959F067-A045-419A-9184-D18B9B7090B2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -676,7 +676,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>134</c:v>
+                  <c:v>424</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>79</c:v>
@@ -685,10 +685,10 @@
                   <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1815,7 +1815,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="O2">
         <f>SUM(O3:O6)</f>
-        <v>134</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="O5">
         <f>SUMPRODUCT(SUMIFS($F$2:$F$36,$H$2:$H$36,M5,$I$2:$I$36,TRUE))</f>
-        <v>0</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="O6">
         <f>SUMPRODUCT(SUMIFS($F$2:$F$37,$H$2:$H$37,M6,$I$2:$I$37,TRUE))</f>
-        <v>0</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2088,7 +2088,7 @@
       </c>
       <c r="O7">
         <f>AVERAGE(O3:O6)</f>
-        <v>33.5</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2227,7 +2227,7 @@
         <v>45978</v>
       </c>
       <c r="I12" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2252,7 +2252,7 @@
         <v>45978</v>
       </c>
       <c r="I13" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2277,7 +2277,7 @@
         <v>45978</v>
       </c>
       <c r="I14" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2302,7 +2302,7 @@
         <v>45978</v>
       </c>
       <c r="I15" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2327,7 +2327,7 @@
         <v>45978</v>
       </c>
       <c r="I16" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2352,7 +2352,7 @@
         <v>45978</v>
       </c>
       <c r="I17" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2377,7 +2377,7 @@
         <v>45978</v>
       </c>
       <c r="I18" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2404,7 +2404,7 @@
         <v>45978</v>
       </c>
       <c r="I19" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2429,7 +2429,7 @@
         <v>45978</v>
       </c>
       <c r="I20" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2454,7 +2454,7 @@
         <v>45978</v>
       </c>
       <c r="I21" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2481,7 +2481,7 @@
         <v>45978</v>
       </c>
       <c r="I22" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2506,7 +2506,7 @@
         <v>45978</v>
       </c>
       <c r="I23" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2531,7 +2531,7 @@
         <v>45978</v>
       </c>
       <c r="I24" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="23.4" x14ac:dyDescent="0.3">
@@ -2560,7 +2560,7 @@
         <v>45978</v>
       </c>
       <c r="I25" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
@@ -2645,7 +2645,7 @@
         <v>45985</v>
       </c>
       <c r="I28" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2670,7 +2670,7 @@
         <v>45985</v>
       </c>
       <c r="I29" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2695,7 +2695,7 @@
         <v>45985</v>
       </c>
       <c r="I30" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2720,7 +2720,7 @@
         <v>45985</v>
       </c>
       <c r="I31" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -2749,7 +2749,7 @@
         <v>45985</v>
       </c>
       <c r="I32" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -2774,7 +2774,7 @@
         <v>45985</v>
       </c>
       <c r="I33" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2799,7 +2799,7 @@
         <v>45985</v>
       </c>
       <c r="I34" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -2824,7 +2824,7 @@
         <v>45985</v>
       </c>
       <c r="I35" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -2849,7 +2849,7 @@
         <v>45985</v>
       </c>
       <c r="I36" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -2874,7 +2874,7 @@
         <v>45985</v>
       </c>
       <c r="I37" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>